<commit_message>
Added Scen_CTax and corrected syntax in Scen_CCS
Scen_CTax has an added scenario for carbon tax based on the 2022 budget speech
</commit_message>
<xml_diff>
--- a/suppxls/Scen_CCS.xlsx
+++ b/suppxls/Scen_CCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C659C9D-1143-493A-AF47-9D06D3030D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0992E247-3159-4AB1-91A1-301F5752AFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="11" xr2:uid="{55565E65-86A1-4E53-88BE-3C00B48900A4}"/>
   </bookViews>
@@ -322,7 +322,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="345">
   <si>
     <t>Comment</t>
   </si>
@@ -10709,10 +10709,10 @@
   <dimension ref="A1:AI36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="7" topLeftCell="V8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="7" topLeftCell="L8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="Z22" sqref="Z22"/>
+      <selection pane="bottomRight" activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10725,13 +10725,11 @@
     <col min="6" max="6" width="10.140625" style="12" customWidth="1"/>
     <col min="7" max="7" width="6.85546875" style="35" customWidth="1"/>
     <col min="8" max="14" width="9.140625" style="12"/>
-    <col min="15" max="22" width="8.5703125" style="12" customWidth="1"/>
+    <col min="15" max="16" width="11.42578125" style="12" customWidth="1"/>
+    <col min="17" max="22" width="8.5703125" style="12" customWidth="1"/>
     <col min="23" max="23" width="9.140625" style="12"/>
     <col min="24" max="24" width="11.42578125" style="12" customWidth="1"/>
-    <col min="25" max="25" width="7.85546875" style="12" customWidth="1"/>
-    <col min="26" max="26" width="7.5703125" style="12" customWidth="1"/>
-    <col min="27" max="28" width="7.85546875" style="12" customWidth="1"/>
-    <col min="29" max="29" width="9.7109375" style="12" customWidth="1"/>
+    <col min="25" max="29" width="10.7109375" style="12" customWidth="1"/>
     <col min="30" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
@@ -11010,7 +11008,7 @@
       </c>
       <c r="W6" s="43"/>
     </row>
-    <row r="7" spans="1:35" s="113" customFormat="1" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" s="113" customFormat="1" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="114" t="s">
         <v>276</v>
       </c>
@@ -11080,20 +11078,25 @@
       <c r="X7" s="112" t="s">
         <v>125</v>
       </c>
-      <c r="Y7" s="114" t="s">
-        <v>126</v>
-      </c>
-      <c r="Z7" s="114" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA7" s="114" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB7" s="114" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC7" s="114" t="s">
-        <v>126</v>
+      <c r="Y7" s="114" t="str">
+        <f>"PRC_ACTFLO~"&amp;Y5</f>
+        <v>PRC_ACTFLO~INMELC</v>
+      </c>
+      <c r="Z7" s="114" t="str">
+        <f t="shared" ref="Z7:AC7" si="0">"PRC_ACTFLO~"&amp;Z5</f>
+        <v>PRC_ACTFLO~INMCEMTHF</v>
+      </c>
+      <c r="AA7" s="114" t="str">
+        <f t="shared" si="0"/>
+        <v>PRC_ACTFLO~IFAELC</v>
+      </c>
+      <c r="AB7" s="114" t="str">
+        <f t="shared" si="0"/>
+        <v>PRC_ACTFLO~ELCC</v>
+      </c>
+      <c r="AC7" s="114" t="str">
+        <f t="shared" si="0"/>
+        <v>PRC_ACTFLO~INMLIMTHF</v>
       </c>
     </row>
     <row r="8" spans="1:35" s="40" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12026,7 +12029,7 @@
       <pane xSplit="3" ySplit="6" topLeftCell="O7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>